<commit_message>
Paper list update August.
</commit_message>
<xml_diff>
--- a/Paper_List.xlsx
+++ b/Paper_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Young Wu\Dropbox\Current\CS799\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Young Wu\Documents\GitHub\MDML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7722958-9469-4E38-B0E1-3CEBD471A254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF408D9E-5F3B-44A7-AEC6-E49BF2CF633A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5137" yWindow="1065" windowWidth="14400" windowHeight="7373" xr2:uid="{E7EE9F80-03A6-4EC3-8DA8-083694855596}"/>
+    <workbookView xWindow="9600" yWindow="1103" windowWidth="9600" windowHeight="7365" xr2:uid="{E7EE9F80-03A6-4EC3-8DA8-083694855596}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -363,6 +363,72 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Causal Strategic Linear Regression</t>
+  </si>
+  <si>
+    <t>https://proceedings.icml.cc/static/paper_files/icml/2020/5468-Paper.pdf</t>
+  </si>
+  <si>
+    <t>Shavit, Edelman, Axelrod</t>
+  </si>
+  <si>
+    <t>Classifiers Induce Invest Effort Strategically</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1807.05307.pdf</t>
+  </si>
+  <si>
+    <t>Kleinberg, Raghavan</t>
+  </si>
+  <si>
+    <t>Linear</t>
+  </si>
+  <si>
+    <t>Strategic Noise in Linear Regression</t>
+  </si>
+  <si>
+    <t>http://www.cs.toronto.edu/~nisarg/papers/equilibria_linreg.pdf</t>
+  </si>
+  <si>
+    <t>Hossain, Shah</t>
+  </si>
+  <si>
+    <t>Lp Norm Minimization</t>
+  </si>
+  <si>
+    <t>Learning Strategy-Aware Linear Classifiers</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/1911.04004.pdf</t>
+  </si>
+  <si>
+    <t>Regret minimization</t>
+  </si>
+  <si>
+    <t>Incentive-Aware PAC Learning</t>
+  </si>
+  <si>
+    <t>https://users.cs.duke.edu/~hrzhang/papers/incentive-aware_learning.pdf</t>
+  </si>
+  <si>
+    <t>Zhang, Conitzer</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Classification with Strategically Withheld Data</t>
+  </si>
+  <si>
+    <t>https://gradanovic.github.io/incentives_in_ML_icml2020_ws/papers/IML2020_paper_13.pdf</t>
+  </si>
+  <si>
+    <t>Krishnaswamy, Li, Rein, Zhang, Conitzer</t>
+  </si>
+  <si>
+    <t>Mincut, Hill-Climbing</t>
   </si>
 </sst>
 </file>
@@ -733,13 +799,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BEFB762-1C7C-4840-8FB5-CF7CC0836E07}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1467,6 +1533,234 @@
       </c>
       <c r="L19" s="1" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="57" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="1">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1489,6 +1783,12 @@
     <hyperlink ref="C17" r:id="rId16" xr:uid="{C28293C0-85A5-4B96-BF35-F99E12BCAF89}"/>
     <hyperlink ref="C18" r:id="rId17" xr:uid="{F687DACA-E137-4C0C-891A-9B065EDD3F16}"/>
     <hyperlink ref="C19" r:id="rId18" xr:uid="{CA647AB7-6B17-463F-B488-33D6F6D12111}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{67360E56-83A8-4864-84A5-151F88C516B8}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{7E8AF9D7-AD35-4331-AE2F-51D71A7F6F40}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{73A47D9C-0EF0-4581-8D04-B749C854956E}"/>
+    <hyperlink ref="C23" r:id="rId22" xr:uid="{97D1F830-BC9D-419D-9560-C1D2F96EF243}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{ABBF34A3-458D-4698-B0EA-7D57E866480C}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{E27BA07E-6551-4979-85CE-6AA36441290B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>